<commit_message>
start some rgee stuff
</commit_message>
<xml_diff>
--- a/FireSurvey/survey/Contact Information.xlsx
+++ b/FireSurvey/survey/Contact Information.xlsx
@@ -11076,56 +11076,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000DEBC3CBCF9AE4458701CB70370E73B7" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95fc3460a10a7b4ed694567eaf15a276">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9d501bca-78b1-4c06-bccc-28d50881c59c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5f188228ccecd6ce7bdd82e135a3b763" ns2:_="">
-    <xsd:import namespace="9d501bca-78b1-4c06-bccc-28d50881c59c"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010051B64F4CAEE3884A936EE11921CD1109" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="294746e90aea9d7e86464dd05a641bc0">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b764bea3eb9b1a5be8fd57fac5fb459b">
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element name="documentManagement">
             <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-              </xsd:all>
+              <xsd:all/>
             </xsd:complexType>
           </xsd:element>
         </xsd:sequence>
       </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9d501bca-78b1-4c06-bccc-28d50881c59c" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="12" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -11242,21 +11204,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F1AF41B-A4E2-462D-9156-287306177EE8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9d501bca-78b1-4c06-bccc-28d50881c59c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D620696-CA10-4891-B8C5-53A9DB4E7351}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>